<commit_message>
Pievienots profila lapas satura dok. + atjaunots darba plāns
</commit_message>
<xml_diff>
--- a/Dok/Proj2_work_plan.xlsx
+++ b/Dok/Proj2_work_plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krists\Documents\GitHub\Arnim\Dok\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KRISTS\DOKUMENTI\STUDIJAS (MAĢISTRS)\Kursi\2. kurss 1. semestris\Kvalifikācijas prakse II\Proj2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>07.09. - 13.09.</t>
   </si>
@@ -122,10 +122,7 @@
     <t>7. IS prezentēšana pasūtītājam</t>
   </si>
   <si>
-    <t>* Jāizdomā, kāda būs profila lapas informācija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    5.3. Profila lapa*</t>
+    <t xml:space="preserve">    5.3. Profila lapa</t>
   </si>
 </sst>
 </file>
@@ -605,7 +602,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U24" sqref="U24"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1257,7 @@
     </row>
     <row r="13" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -1888,8 +1885,8 @@
       <c r="R23" s="16"/>
       <c r="S23" s="16"/>
       <c r="T23" s="16"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="15"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
       <c r="W23" s="15"/>
       <c r="X23" s="15"/>
       <c r="Y23" s="15"/>
@@ -2013,9 +2010,7 @@
       <c r="BS24" s="2"/>
     </row>
     <row r="25" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="A25" s="7"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>

</xml_diff>